<commit_message>
Need to see about missing data in result file
</commit_message>
<xml_diff>
--- a/Assignments/Project4/Expectation Analysis.xlsx
+++ b/Assignments/Project4/Expectation Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91D6CF9-B979-4C5B-B1A5-FEE62AE587AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A6114-BA6E-4262-98C9-4D4AB5A85842}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="700" activeTab="3" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal" sheetId="12" r:id="rId1"/>
@@ -540,7 +540,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="174" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1657,7 +1657,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="280">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2284,75 +2284,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2372,7 +2303,85 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2694,8 +2703,8 @@
   </sheetPr>
   <dimension ref="A1:AM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40"/>
+    <sheetView topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,28 +2749,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="244" t="s">
+      <c r="J1" s="254" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="244"/>
-      <c r="L1" s="244"/>
-      <c r="M1" s="244"/>
-      <c r="N1" s="244"/>
-      <c r="O1" s="244"/>
-      <c r="P1" s="244"/>
-      <c r="Q1" s="244"/>
-      <c r="R1" s="244"/>
-      <c r="S1" s="244"/>
-      <c r="T1" s="244"/>
-      <c r="U1" s="244"/>
-      <c r="V1" s="244"/>
-      <c r="W1" s="244"/>
-      <c r="X1" s="244"/>
-      <c r="Y1" s="244"/>
-      <c r="Z1" s="244"/>
-      <c r="AA1" s="244"/>
-      <c r="AB1" s="244"/>
-      <c r="AC1" s="244"/>
+      <c r="K1" s="254"/>
+      <c r="L1" s="254"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="254"/>
+      <c r="O1" s="254"/>
+      <c r="P1" s="254"/>
+      <c r="Q1" s="254"/>
+      <c r="R1" s="254"/>
+      <c r="S1" s="254"/>
+      <c r="T1" s="254"/>
+      <c r="U1" s="254"/>
+      <c r="V1" s="254"/>
+      <c r="W1" s="254"/>
+      <c r="X1" s="254"/>
+      <c r="Y1" s="254"/>
+      <c r="Z1" s="254"/>
+      <c r="AA1" s="254"/>
+      <c r="AB1" s="254"/>
+      <c r="AC1" s="254"/>
     </row>
     <row r="2" spans="1:38" s="116" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="95" t="s">
@@ -2881,7 +2890,7 @@
         <f>S3/(T3-S3)</f>
         <v>48.37461300309613</v>
       </c>
-      <c r="V3" s="267">
+      <c r="V3" s="244">
         <f>D21*1000/(3*10^8)</f>
         <v>4.6666666666666669E-2</v>
       </c>
@@ -2962,7 +2971,7 @@
         <f t="shared" ref="U4:U12" si="2">S4/(T4-S4)</f>
         <v>1</v>
       </c>
-      <c r="V4" s="268">
+      <c r="V4" s="245">
         <f>E21*1000/(3*10^8)</f>
         <v>2.6333333333333334E-2</v>
       </c>
@@ -3043,7 +3052,7 @@
         <f t="shared" si="2"/>
         <v>0.47528517110266161</v>
       </c>
-      <c r="V5" s="269">
+      <c r="V5" s="246">
         <f>F21*1000/(3*10^8)</f>
         <v>0.04</v>
       </c>
@@ -3124,7 +3133,7 @@
         <f t="shared" si="2"/>
         <v>0.47528517110266161</v>
       </c>
-      <c r="V6" s="268">
+      <c r="V6" s="245">
         <f>B22*1000/(3*10^8)</f>
         <v>1.7999999999999999E-2</v>
       </c>
@@ -3205,7 +3214,7 @@
         <f t="shared" si="2"/>
         <v>1.8115942028985508</v>
       </c>
-      <c r="V7" s="269">
+      <c r="V7" s="246">
         <f>D22*1000/(3*10^8)</f>
         <v>4.1666666666666664E-2</v>
       </c>
@@ -3280,7 +3289,7 @@
         <f t="shared" si="2"/>
         <v>1.8115942028985508</v>
       </c>
-      <c r="V8" s="268">
+      <c r="V8" s="245">
         <f>E23*1000/(3*10^8)</f>
         <v>3.7333333333333336E-2</v>
       </c>
@@ -3366,7 +3375,7 @@
         <f t="shared" si="2"/>
         <v>1.2667207134171057</v>
       </c>
-      <c r="V9" s="269">
+      <c r="V9" s="246">
         <f>F23*1000/(3*10^8)</f>
         <v>1.5333333333333332E-2</v>
       </c>
@@ -3458,7 +3467,7 @@
         <f t="shared" si="2"/>
         <v>1.8115942028985508</v>
       </c>
-      <c r="V10" s="268">
+      <c r="V10" s="245">
         <f>C24*1000/(3*10^8)</f>
         <v>8.3333333333333332E-3</v>
       </c>
@@ -3554,7 +3563,7 @@
         <f t="shared" si="2"/>
         <v>8.4459459459459438</v>
       </c>
-      <c r="V11" s="270">
+      <c r="V11" s="247">
         <f>C25*1000/(3*10^8)</f>
         <v>2.7333333333333334E-2</v>
       </c>
@@ -3649,7 +3658,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="V12" s="271">
+      <c r="V12" s="248">
         <f>E25*1000/(3*10^8)</f>
         <v>2.1999999999999999E-2</v>
       </c>
@@ -3987,7 +3996,7 @@
         <f>L18/(M18-L18)</f>
         <v>0.10861631503944945</v>
       </c>
-      <c r="O18" s="272">
+      <c r="O18" s="249">
         <f t="shared" ref="O18:O27" si="7">V3</f>
         <v>4.6666666666666669E-2</v>
       </c>
@@ -4022,16 +4031,16 @@
       <c r="AL18" s="119"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="246" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="248" t="s">
+      <c r="A19" s="256" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="258" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="249"/>
-      <c r="D19" s="249"/>
-      <c r="E19" s="249"/>
-      <c r="F19" s="250"/>
+      <c r="C19" s="259"/>
+      <c r="D19" s="259"/>
+      <c r="E19" s="259"/>
+      <c r="F19" s="260"/>
       <c r="G19" s="55"/>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
@@ -4052,7 +4061,7 @@
         <f t="shared" ref="N19:N27" si="10">L19/(M19-L19)</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="O19" s="273">
+      <c r="O19" s="250">
         <f t="shared" si="7"/>
         <v>2.6333333333333334E-2</v>
       </c>
@@ -4087,7 +4096,7 @@
       <c r="AL19" s="119"/>
     </row>
     <row r="20" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="247"/>
+      <c r="A20" s="257"/>
       <c r="B20" s="98" t="s">
         <v>2</v>
       </c>
@@ -4123,7 +4132,7 @@
         <f t="shared" si="10"/>
         <v>0.47528517110266161</v>
       </c>
-      <c r="O20" s="272">
+      <c r="O20" s="249">
         <f t="shared" si="7"/>
         <v>0.04</v>
       </c>
@@ -4196,7 +4205,7 @@
         <f t="shared" si="10"/>
         <v>0.34722222222222221</v>
       </c>
-      <c r="O21" s="273">
+      <c r="O21" s="250">
         <f t="shared" si="7"/>
         <v>1.7999999999999999E-2</v>
       </c>
@@ -4220,10 +4229,10 @@
         <f t="shared" si="12"/>
         <v>2.0618556701030927E-2</v>
       </c>
-      <c r="Z21" s="256" t="s">
+      <c r="Z21" s="266" t="s">
         <v>70</v>
       </c>
-      <c r="AA21" s="257"/>
+      <c r="AA21" s="267"/>
       <c r="AD21" s="119"/>
       <c r="AF21" s="119"/>
       <c r="AG21" s="119"/>
@@ -4272,7 +4281,7 @@
         <f t="shared" si="10"/>
         <v>1.8115942028985508</v>
       </c>
-      <c r="O22" s="272">
+      <c r="O22" s="249">
         <f t="shared" si="7"/>
         <v>4.1666666666666664E-2</v>
       </c>
@@ -4351,7 +4360,7 @@
         <f t="shared" si="10"/>
         <v>1.8115942028985508</v>
       </c>
-      <c r="O23" s="273">
+      <c r="O23" s="250">
         <f t="shared" si="7"/>
         <v>3.7333333333333336E-2</v>
       </c>
@@ -4429,7 +4438,7 @@
         <f t="shared" si="10"/>
         <v>1.2667207134171057</v>
       </c>
-      <c r="O24" s="272">
+      <c r="O24" s="249">
         <f t="shared" si="7"/>
         <v>1.5333333333333332E-2</v>
       </c>
@@ -4508,7 +4517,7 @@
         <f t="shared" si="10"/>
         <v>0.47528517110266161</v>
       </c>
-      <c r="O25" s="273">
+      <c r="O25" s="250">
         <f t="shared" si="7"/>
         <v>8.3333333333333332E-3</v>
       </c>
@@ -4572,7 +4581,7 @@
         <f t="shared" si="10"/>
         <v>0.28788576692768308</v>
       </c>
-      <c r="O26" s="272">
+      <c r="O26" s="249">
         <f t="shared" si="7"/>
         <v>2.7333333333333334E-2</v>
       </c>
@@ -4625,7 +4634,7 @@
         <f t="shared" si="10"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="O27" s="274">
+      <c r="O27" s="251">
         <f t="shared" si="7"/>
         <v>2.1999999999999999E-2</v>
       </c>
@@ -4660,16 +4669,16 @@
       <c r="AM27" s="119"/>
     </row>
     <row r="28" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="254" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="251" t="s">
+      <c r="A28" s="264" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="261" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="252"/>
-      <c r="D28" s="252"/>
-      <c r="E28" s="252"/>
-      <c r="F28" s="253"/>
+      <c r="C28" s="262"/>
+      <c r="D28" s="262"/>
+      <c r="E28" s="262"/>
+      <c r="F28" s="263"/>
       <c r="K28" s="143" t="s">
         <v>121</v>
       </c>
@@ -4695,7 +4704,7 @@
       <c r="AH28" s="119"/>
     </row>
     <row r="29" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="255"/>
+      <c r="A29" s="265"/>
       <c r="B29" s="139" t="s">
         <v>2</v>
       </c>
@@ -4755,13 +4764,13 @@
       <c r="F31" s="113">
         <v>50</v>
       </c>
-      <c r="K31" s="245" t="s">
+      <c r="K31" s="255" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="245"/>
-      <c r="M31" s="245"/>
-      <c r="N31" s="245"/>
-      <c r="O31" s="245"/>
+      <c r="L31" s="255"/>
+      <c r="M31" s="255"/>
+      <c r="N31" s="255"/>
+      <c r="O31" s="255"/>
       <c r="P31" s="119"/>
       <c r="Q31" s="119"/>
       <c r="AG31" s="119"/>
@@ -5179,7 +5188,7 @@
       <c r="B43" s="55"/>
       <c r="C43" s="134"/>
       <c r="D43" s="134"/>
-      <c r="G43" s="275"/>
+      <c r="G43" s="252"/>
       <c r="K43" s="119" t="s">
         <v>80</v>
       </c>
@@ -6677,13 +6686,13 @@
       <c r="D15" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="245" t="s">
+      <c r="J15" s="255" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="245"/>
-      <c r="L15" s="245"/>
-      <c r="M15" s="245"/>
-      <c r="N15" s="245"/>
+      <c r="K15" s="255"/>
+      <c r="L15" s="255"/>
+      <c r="M15" s="255"/>
+      <c r="N15" s="255"/>
       <c r="O15" s="56"/>
       <c r="P15" s="56"/>
       <c r="Q15" s="56"/>
@@ -6789,16 +6798,16 @@
       <c r="AL17" s="56"/>
     </row>
     <row r="18" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="260" t="s">
+      <c r="A18" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="261"/>
-      <c r="D18" s="261"/>
-      <c r="E18" s="261"/>
-      <c r="F18" s="262"/>
+      <c r="C18" s="271"/>
+      <c r="D18" s="271"/>
+      <c r="E18" s="271"/>
+      <c r="F18" s="272"/>
       <c r="G18" s="55"/>
       <c r="H18" s="55"/>
       <c r="I18" s="55"/>
@@ -6821,7 +6830,7 @@
       <c r="AL18" s="56"/>
     </row>
     <row r="19" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="259"/>
+      <c r="A19" s="269"/>
       <c r="B19" s="18" t="s">
         <v>2</v>
       </c>
@@ -8104,34 +8113,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="260" t="s">
+      <c r="A1" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="261"/>
-      <c r="D1" s="261"/>
-      <c r="E1" s="261"/>
-      <c r="F1" s="262"/>
-      <c r="H1" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="260" t="s">
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="272"/>
+      <c r="H1" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="261"/>
-      <c r="K1" s="261"/>
-      <c r="L1" s="261"/>
-      <c r="M1" s="262"/>
-      <c r="O1" s="263" t="s">
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="272"/>
+      <c r="O1" s="273" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="263"/>
-      <c r="Q1" s="263"/>
+      <c r="P1" s="273"/>
+      <c r="Q1" s="273"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="266"/>
+      <c r="A2" s="276"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -8148,7 +8157,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="266"/>
+      <c r="H2" s="276"/>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -8418,26 +8427,26 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="264" t="s">
+      <c r="A8" s="274" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="264"/>
-      <c r="C8" s="264"/>
-      <c r="D8" s="264"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
+      <c r="B8" s="274"/>
+      <c r="C8" s="274"/>
+      <c r="D8" s="274"/>
+      <c r="E8" s="274"/>
+      <c r="F8" s="274"/>
       <c r="G8">
         <f>SUM(B3:F7)</f>
         <v>9700</v>
       </c>
-      <c r="H8" s="264" t="s">
+      <c r="H8" s="274" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="265"/>
-      <c r="J8" s="265"/>
-      <c r="K8" s="265"/>
-      <c r="L8" s="265"/>
-      <c r="M8" s="265"/>
+      <c r="I8" s="275"/>
+      <c r="J8" s="275"/>
+      <c r="K8" s="275"/>
+      <c r="L8" s="275"/>
+      <c r="M8" s="275"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9">
@@ -8467,16 +8476,16 @@
       <c r="N9" s="223"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="260" t="s">
+      <c r="A10" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="261"/>
-      <c r="D10" s="261"/>
-      <c r="E10" s="261"/>
-      <c r="F10" s="262"/>
+      <c r="C10" s="271"/>
+      <c r="D10" s="271"/>
+      <c r="E10" s="271"/>
+      <c r="F10" s="272"/>
       <c r="I10" s="223"/>
       <c r="J10" s="223"/>
       <c r="K10" s="223"/>
@@ -8484,7 +8493,7 @@
       <c r="M10" s="223"/>
     </row>
     <row r="11" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="259"/>
+      <c r="A11" s="269"/>
       <c r="B11" s="18" t="s">
         <v>2</v>
       </c>
@@ -8525,16 +8534,16 @@
       <c r="F12" s="9">
         <v>12000</v>
       </c>
-      <c r="H12" s="258" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="260" t="s">
+      <c r="H12" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="270" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="261"/>
-      <c r="K12" s="261"/>
-      <c r="L12" s="261"/>
-      <c r="M12" s="262"/>
+      <c r="J12" s="271"/>
+      <c r="K12" s="271"/>
+      <c r="L12" s="271"/>
+      <c r="M12" s="272"/>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -8556,7 +8565,7 @@
         <v>8200</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="266"/>
+      <c r="H13" s="276"/>
       <c r="I13" s="50" t="s">
         <v>2</v>
       </c>
@@ -8706,14 +8715,14 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="264" t="s">
+      <c r="A17" s="274" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="264"/>
-      <c r="C17" s="264"/>
-      <c r="D17" s="264"/>
-      <c r="E17" s="264"/>
-      <c r="F17" s="264"/>
+      <c r="B17" s="274"/>
+      <c r="C17" s="274"/>
+      <c r="D17" s="274"/>
+      <c r="E17" s="274"/>
+      <c r="F17" s="274"/>
       <c r="H17" s="10" t="s">
         <v>5</v>
       </c>
@@ -8777,14 +8786,14 @@
         <v>20</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="H19" s="264" t="s">
+      <c r="H19" s="274" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="264"/>
-      <c r="J19" s="264"/>
-      <c r="K19" s="264"/>
-      <c r="L19" s="264"/>
-      <c r="M19" s="264"/>
+      <c r="I19" s="274"/>
+      <c r="J19" s="274"/>
+      <c r="K19" s="274"/>
+      <c r="L19" s="274"/>
+      <c r="M19" s="274"/>
     </row>
     <row r="20" spans="1:13" ht="52.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -8925,12 +8934,12 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="264" t="s">
+      <c r="A27" s="274" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="264"/>
-      <c r="C27" s="264"/>
-      <c r="D27" s="264"/>
+      <c r="B27" s="274"/>
+      <c r="C27" s="274"/>
+      <c r="D27" s="274"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
     </row>
@@ -8957,10 +8966,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DBAA6-739A-4660-96E4-A6E1D48EB2A8}">
-  <dimension ref="D2:K36"/>
+  <dimension ref="D2:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8970,9 +8979,11 @@
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D2" s="224" t="s">
         <v>0</v>
       </c>
@@ -8985,7 +8996,7 @@
       <c r="I2" s="224"/>
       <c r="J2" s="224"/>
     </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D3" s="224"/>
       <c r="E3" s="224" t="s">
         <v>2</v>
@@ -9003,8 +9014,10 @@
         <v>6</v>
       </c>
       <c r="J3" s="224"/>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O3" s="224"/>
+      <c r="P3" s="224"/>
+    </row>
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D4" s="224" t="s">
         <v>2</v>
       </c>
@@ -9026,8 +9039,11 @@
       <c r="J4" s="224">
         <v>0.40721649484536082</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O4" s="227"/>
+      <c r="P4" s="277"/>
+      <c r="Q4" s="243"/>
+    </row>
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D5" s="224" t="s">
         <v>3</v>
       </c>
@@ -9053,8 +9069,11 @@
         <f>J4+J5</f>
         <v>0.51546391752577314</v>
       </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O5" s="35"/>
+      <c r="P5" s="278"/>
+      <c r="Q5" s="243"/>
+    </row>
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D6" s="224" t="s">
         <v>4</v>
       </c>
@@ -9080,8 +9099,11 @@
         <f>K5+J6</f>
         <v>0.67010309278350511</v>
       </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O6" s="35"/>
+      <c r="P6" s="278"/>
+      <c r="Q6" s="243"/>
+    </row>
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D7" s="224" t="s">
         <v>5</v>
       </c>
@@ -9107,8 +9129,11 @@
         <f t="shared" ref="K7:K8" si="0">K6+J7</f>
         <v>0.82474226804123707</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O7" s="35"/>
+      <c r="P7" s="278"/>
+      <c r="Q7" s="243"/>
+    </row>
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D8" s="224" t="s">
         <v>6</v>
       </c>
@@ -9134,8 +9159,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="O8" s="225"/>
+      <c r="P8" s="279"/>
+    </row>
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D9" s="224"/>
       <c r="E9" s="224"/>
       <c r="F9" s="224"/>
@@ -9144,7 +9171,7 @@
       <c r="I9" s="224"/>
       <c r="J9" s="224"/>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D10" s="224"/>
       <c r="E10" s="224"/>
       <c r="F10" s="224"/>
@@ -9153,12 +9180,12 @@
       <c r="I10" s="224"/>
       <c r="J10" s="224"/>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D11" s="242" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>0</v>
       </c>
@@ -9181,7 +9208,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>2</v>
       </c>
@@ -9210,7 +9237,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>3</v>
       </c>
@@ -9239,7 +9266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -9268,7 +9295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -9476,7 +9503,7 @@
       <c r="F27" s="194">
         <v>2551.6799999999998</v>
       </c>
-      <c r="G27" s="276">
+      <c r="G27" s="253">
         <f>1/F27*1000</f>
         <v>0.39189867067970907</v>
       </c>
@@ -9491,7 +9518,7 @@
       <c r="F28" s="105">
         <v>2000</v>
       </c>
-      <c r="G28" s="276">
+      <c r="G28" s="253">
         <f t="shared" ref="G28:G36" si="13">1/F28*1000</f>
         <v>0.5</v>
       </c>
@@ -9506,7 +9533,7 @@
       <c r="F29" s="194">
         <v>776</v>
       </c>
-      <c r="G29" s="276">
+      <c r="G29" s="253">
         <f t="shared" si="13"/>
         <v>1.2886597938144331</v>
       </c>
@@ -9521,7 +9548,7 @@
       <c r="F30" s="105">
         <v>776</v>
       </c>
-      <c r="G30" s="276">
+      <c r="G30" s="253">
         <f t="shared" si="13"/>
         <v>1.2886597938144331</v>
       </c>
@@ -9536,7 +9563,7 @@
       <c r="F31" s="194">
         <v>776</v>
       </c>
-      <c r="G31" s="276">
+      <c r="G31" s="253">
         <f t="shared" si="13"/>
         <v>1.2886597938144331</v>
       </c>
@@ -9551,7 +9578,7 @@
       <c r="F32" s="105">
         <v>776</v>
       </c>
-      <c r="G32" s="276">
+      <c r="G32" s="253">
         <f t="shared" si="13"/>
         <v>1.2886597938144331</v>
       </c>
@@ -9566,7 +9593,7 @@
       <c r="F33" s="194">
         <v>447.36</v>
       </c>
-      <c r="G33" s="276">
+      <c r="G33" s="253">
         <f t="shared" si="13"/>
         <v>2.2353361945636623</v>
       </c>
@@ -9581,7 +9608,7 @@
       <c r="F34" s="105">
         <v>776</v>
       </c>
-      <c r="G34" s="276">
+      <c r="G34" s="253">
         <f t="shared" si="13"/>
         <v>1.2886597938144331</v>
       </c>
@@ -9596,7 +9623,7 @@
       <c r="F35" s="194">
         <v>223.68</v>
       </c>
-      <c r="G35" s="276">
+      <c r="G35" s="253">
         <f t="shared" si="13"/>
         <v>4.4706723891273246</v>
       </c>
@@ -9611,7 +9638,7 @@
       <c r="F36" s="124">
         <v>2000</v>
       </c>
-      <c r="G36" s="276">
+      <c r="G36" s="253">
         <f t="shared" si="13"/>
         <v>0.5</v>
       </c>

</xml_diff>

<commit_message>
Need to work on the analysis
</commit_message>
<xml_diff>
--- a/Assignments/Project4/Expectation Analysis.xlsx
+++ b/Assignments/Project4/Expectation Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A6114-BA6E-4262-98C9-4D4AB5A85842}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE2A0D8-37C3-4174-A169-928BA097FD96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="700" activeTab="3" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal" sheetId="12" r:id="rId1"/>
@@ -536,11 +536,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1657,7 +1658,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="280">
+  <cellXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2304,6 +2305,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2372,15 +2383,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="84" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2703,8 +2705,8 @@
   </sheetPr>
   <dimension ref="A1:AM69"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2735,9 +2737,9 @@
     <col min="25" max="25" width="11.85546875" style="118" customWidth="1"/>
     <col min="26" max="26" width="21.7109375" style="118" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.85546875" style="118" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" style="118" customWidth="1"/>
-    <col min="29" max="29" width="10.7109375" style="118" customWidth="1"/>
-    <col min="30" max="30" width="10" style="118" customWidth="1"/>
+    <col min="28" max="28" width="40.28515625" style="118" customWidth="1"/>
+    <col min="29" max="29" width="20.7109375" style="118" customWidth="1"/>
+    <col min="30" max="30" width="15.28515625" style="118" customWidth="1"/>
     <col min="31" max="31" width="34.42578125" style="118" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="18.5703125" style="118" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10.7109375" style="118" bestFit="1" customWidth="1"/>
@@ -2749,28 +2751,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="254" t="s">
+      <c r="J1" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="254"/>
-      <c r="L1" s="254"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="254"/>
-      <c r="O1" s="254"/>
-      <c r="P1" s="254"/>
-      <c r="Q1" s="254"/>
-      <c r="R1" s="254"/>
-      <c r="S1" s="254"/>
-      <c r="T1" s="254"/>
-      <c r="U1" s="254"/>
-      <c r="V1" s="254"/>
-      <c r="W1" s="254"/>
-      <c r="X1" s="254"/>
-      <c r="Y1" s="254"/>
-      <c r="Z1" s="254"/>
-      <c r="AA1" s="254"/>
-      <c r="AB1" s="254"/>
-      <c r="AC1" s="254"/>
+      <c r="K1" s="258"/>
+      <c r="L1" s="258"/>
+      <c r="M1" s="258"/>
+      <c r="N1" s="258"/>
+      <c r="O1" s="258"/>
+      <c r="P1" s="258"/>
+      <c r="Q1" s="258"/>
+      <c r="R1" s="258"/>
+      <c r="S1" s="258"/>
+      <c r="T1" s="258"/>
+      <c r="U1" s="258"/>
+      <c r="V1" s="258"/>
+      <c r="W1" s="258"/>
+      <c r="X1" s="258"/>
+      <c r="Y1" s="258"/>
+      <c r="Z1" s="258"/>
+      <c r="AA1" s="258"/>
+      <c r="AB1" s="258"/>
+      <c r="AC1" s="258"/>
     </row>
     <row r="2" spans="1:38" s="116" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="95" t="s">
@@ -4020,6 +4022,7 @@
         <f>L18/($L$28+$S$13)</f>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V18" s="119"/>
       <c r="AD18" s="119"/>
       <c r="AE18" s="119"/>
       <c r="AF18" s="119"/>
@@ -4031,16 +4034,16 @@
       <c r="AL18" s="119"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="256" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="258" t="s">
+      <c r="A19" s="260" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="262" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="259"/>
-      <c r="D19" s="259"/>
-      <c r="E19" s="259"/>
-      <c r="F19" s="260"/>
+      <c r="C19" s="263"/>
+      <c r="D19" s="263"/>
+      <c r="E19" s="263"/>
+      <c r="F19" s="264"/>
       <c r="G19" s="55"/>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
@@ -4085,6 +4088,7 @@
         <f t="shared" ref="T19:T27" si="12">L19/($L$28+$S$13)</f>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V19" s="119"/>
       <c r="AD19" s="119"/>
       <c r="AE19" s="119"/>
       <c r="AF19" s="119"/>
@@ -4096,7 +4100,7 @@
       <c r="AL19" s="119"/>
     </row>
     <row r="20" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="257"/>
+      <c r="A20" s="261"/>
       <c r="B20" s="98" t="s">
         <v>2</v>
       </c>
@@ -4156,6 +4160,7 @@
         <f t="shared" si="12"/>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V20" s="119"/>
       <c r="AD20" s="119"/>
       <c r="AE20" s="119"/>
       <c r="AF20" s="119"/>
@@ -4229,10 +4234,11 @@
         <f t="shared" si="12"/>
         <v>2.0618556701030927E-2</v>
       </c>
-      <c r="Z21" s="266" t="s">
+      <c r="V21" s="119"/>
+      <c r="Z21" s="270" t="s">
         <v>70</v>
       </c>
-      <c r="AA21" s="267"/>
+      <c r="AA21" s="271"/>
       <c r="AD21" s="119"/>
       <c r="AF21" s="119"/>
       <c r="AG21" s="119"/>
@@ -4305,6 +4311,7 @@
         <f t="shared" si="12"/>
         <v>5.1546391752577317E-2</v>
       </c>
+      <c r="V22" s="119"/>
       <c r="Z22" s="105" t="s">
         <v>71</v>
       </c>
@@ -4384,6 +4391,7 @@
         <f t="shared" si="12"/>
         <v>5.1546391752577317E-2</v>
       </c>
+      <c r="V23" s="119"/>
       <c r="Z23" s="105" t="s">
         <v>72</v>
       </c>
@@ -4462,6 +4470,7 @@
         <f t="shared" si="12"/>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V24" s="119"/>
       <c r="Z24" s="105" t="s">
         <v>106</v>
       </c>
@@ -4541,6 +4550,7 @@
         <f t="shared" si="12"/>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V25" s="119"/>
       <c r="Z25" s="105" t="s">
         <v>73</v>
       </c>
@@ -4605,6 +4615,7 @@
         <f t="shared" si="12"/>
         <v>5.1546391752577319E-3</v>
       </c>
+      <c r="V26" s="119"/>
       <c r="AE26" s="119"/>
       <c r="AF26" s="119"/>
       <c r="AG26" s="119"/>
@@ -4658,6 +4669,7 @@
         <f t="shared" si="12"/>
         <v>2.5773195876288658E-2</v>
       </c>
+      <c r="V27" s="119"/>
       <c r="AE27" s="119"/>
       <c r="AF27" s="119"/>
       <c r="AG27" s="119"/>
@@ -4669,16 +4681,16 @@
       <c r="AM27" s="119"/>
     </row>
     <row r="28" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="264" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="261" t="s">
+      <c r="A28" s="268" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="265" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="262"/>
-      <c r="D28" s="262"/>
-      <c r="E28" s="262"/>
-      <c r="F28" s="263"/>
+      <c r="C28" s="266"/>
+      <c r="D28" s="266"/>
+      <c r="E28" s="266"/>
+      <c r="F28" s="267"/>
       <c r="K28" s="143" t="s">
         <v>121</v>
       </c>
@@ -4704,7 +4716,7 @@
       <c r="AH28" s="119"/>
     </row>
     <row r="29" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="265"/>
+      <c r="A29" s="269"/>
       <c r="B29" s="139" t="s">
         <v>2</v>
       </c>
@@ -4720,8 +4732,8 @@
       <c r="F29" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="AG29" s="119"/>
-      <c r="AH29" s="119"/>
+      <c r="AE29" s="119"/>
+      <c r="AF29" s="119"/>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" s="163" t="s">
@@ -4742,8 +4754,8 @@
       <c r="F30" s="111">
         <v>250</v>
       </c>
+      <c r="AF30" s="119"/>
       <c r="AG30" s="119"/>
-      <c r="AH30" s="119"/>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" s="140" t="s">
@@ -4764,17 +4776,17 @@
       <c r="F31" s="113">
         <v>50</v>
       </c>
-      <c r="K31" s="255" t="s">
+      <c r="K31" s="259" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="255"/>
-      <c r="M31" s="255"/>
-      <c r="N31" s="255"/>
-      <c r="O31" s="255"/>
+      <c r="L31" s="259"/>
+      <c r="M31" s="259"/>
+      <c r="N31" s="259"/>
+      <c r="O31" s="259"/>
       <c r="P31" s="119"/>
       <c r="Q31" s="119"/>
+      <c r="AF31" s="119"/>
       <c r="AG31" s="119"/>
-      <c r="AH31" s="119"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" s="140" t="s">
@@ -4811,8 +4823,8 @@
       </c>
       <c r="P32" s="119"/>
       <c r="Q32" s="119"/>
+      <c r="AF32" s="119"/>
       <c r="AG32" s="119"/>
-      <c r="AH32" s="119"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="140" t="s">
@@ -5415,8 +5427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEFF1FD-2D58-4EC4-935B-23EC7B50B19C}">
   <dimension ref="A1:AM62"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+    <sheetView topLeftCell="F1" zoomScale="64" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AE37" sqref="AE37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6686,13 +6698,13 @@
       <c r="D15" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="255" t="s">
+      <c r="J15" s="259" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="255"/>
-      <c r="L15" s="255"/>
-      <c r="M15" s="255"/>
-      <c r="N15" s="255"/>
+      <c r="K15" s="259"/>
+      <c r="L15" s="259"/>
+      <c r="M15" s="259"/>
+      <c r="N15" s="259"/>
       <c r="O15" s="56"/>
       <c r="P15" s="56"/>
       <c r="Q15" s="56"/>
@@ -6798,16 +6810,16 @@
       <c r="AL17" s="56"/>
     </row>
     <row r="18" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="270" t="s">
+      <c r="A18" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="274" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="271"/>
-      <c r="D18" s="271"/>
-      <c r="E18" s="271"/>
-      <c r="F18" s="272"/>
+      <c r="C18" s="275"/>
+      <c r="D18" s="275"/>
+      <c r="E18" s="275"/>
+      <c r="F18" s="276"/>
       <c r="G18" s="55"/>
       <c r="H18" s="55"/>
       <c r="I18" s="55"/>
@@ -6830,7 +6842,7 @@
       <c r="AL18" s="56"/>
     </row>
     <row r="19" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="269"/>
+      <c r="A19" s="273"/>
       <c r="B19" s="18" t="s">
         <v>2</v>
       </c>
@@ -8099,7 +8111,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G3" sqref="G3:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8113,34 +8125,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="270" t="s">
+      <c r="A1" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="274" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="272"/>
-      <c r="H1" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="270" t="s">
+      <c r="C1" s="275"/>
+      <c r="D1" s="275"/>
+      <c r="E1" s="275"/>
+      <c r="F1" s="276"/>
+      <c r="H1" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="274" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="272"/>
-      <c r="O1" s="273" t="s">
+      <c r="J1" s="275"/>
+      <c r="K1" s="275"/>
+      <c r="L1" s="275"/>
+      <c r="M1" s="276"/>
+      <c r="O1" s="277" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="273"/>
+      <c r="P1" s="277"/>
+      <c r="Q1" s="277"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="276"/>
+      <c r="A2" s="280"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -8157,7 +8169,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="276"/>
+      <c r="H2" s="280"/>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -8427,32 +8439,25 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="274" t="s">
+      <c r="A8" s="278" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="274"/>
-      <c r="C8" s="274"/>
-      <c r="D8" s="274"/>
-      <c r="E8" s="274"/>
-      <c r="F8" s="274"/>
-      <c r="G8">
-        <f>SUM(B3:F7)</f>
-        <v>9700</v>
-      </c>
-      <c r="H8" s="274" t="s">
+      <c r="B8" s="278"/>
+      <c r="C8" s="278"/>
+      <c r="D8" s="278"/>
+      <c r="E8" s="278"/>
+      <c r="F8" s="278"/>
+      <c r="H8" s="278" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="275"/>
-      <c r="J8" s="275"/>
-      <c r="K8" s="275"/>
-      <c r="L8" s="275"/>
-      <c r="M8" s="275"/>
+      <c r="I8" s="279"/>
+      <c r="J8" s="279"/>
+      <c r="K8" s="279"/>
+      <c r="L8" s="279"/>
+      <c r="M8" s="279"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G9">
-        <f>1/G8*1000</f>
-        <v>0.10309278350515465</v>
-      </c>
+      <c r="G9" s="257"/>
       <c r="I9" s="223">
         <f>SUM(I3:I7)</f>
         <v>0.10309278350515463</v>
@@ -8476,16 +8481,17 @@
       <c r="N9" s="223"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="270" t="s">
+      <c r="A10" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="274" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="271"/>
-      <c r="D10" s="271"/>
-      <c r="E10" s="271"/>
-      <c r="F10" s="272"/>
+      <c r="C10" s="275"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="276"/>
+      <c r="G10" s="257"/>
       <c r="I10" s="223"/>
       <c r="J10" s="223"/>
       <c r="K10" s="223"/>
@@ -8493,7 +8499,7 @@
       <c r="M10" s="223"/>
     </row>
     <row r="11" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="269"/>
+      <c r="A11" s="273"/>
       <c r="B11" s="18" t="s">
         <v>2</v>
       </c>
@@ -8509,6 +8515,7 @@
       <c r="F11" s="19" t="s">
         <v>6</v>
       </c>
+      <c r="G11" s="257"/>
       <c r="I11" s="223"/>
       <c r="J11" s="223"/>
       <c r="K11" s="223"/>
@@ -8534,16 +8541,17 @@
       <c r="F12" s="9">
         <v>12000</v>
       </c>
-      <c r="H12" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="270" t="s">
+      <c r="G12" s="257"/>
+      <c r="H12" s="272" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="274" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="271"/>
-      <c r="K12" s="271"/>
-      <c r="L12" s="271"/>
-      <c r="M12" s="272"/>
+      <c r="J12" s="275"/>
+      <c r="K12" s="275"/>
+      <c r="L12" s="275"/>
+      <c r="M12" s="276"/>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -8564,8 +8572,8 @@
       <c r="F13" s="1">
         <v>8200</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="276"/>
+      <c r="G13" s="257"/>
+      <c r="H13" s="280"/>
       <c r="I13" s="50" t="s">
         <v>2</v>
       </c>
@@ -8715,14 +8723,14 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="274" t="s">
+      <c r="A17" s="278" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="274"/>
-      <c r="C17" s="274"/>
-      <c r="D17" s="274"/>
-      <c r="E17" s="274"/>
-      <c r="F17" s="274"/>
+      <c r="B17" s="278"/>
+      <c r="C17" s="278"/>
+      <c r="D17" s="278"/>
+      <c r="E17" s="278"/>
+      <c r="F17" s="278"/>
       <c r="H17" s="10" t="s">
         <v>5</v>
       </c>
@@ -8786,14 +8794,14 @@
         <v>20</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="H19" s="274" t="s">
+      <c r="H19" s="278" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="274"/>
-      <c r="J19" s="274"/>
-      <c r="K19" s="274"/>
-      <c r="L19" s="274"/>
-      <c r="M19" s="274"/>
+      <c r="I19" s="278"/>
+      <c r="J19" s="278"/>
+      <c r="K19" s="278"/>
+      <c r="L19" s="278"/>
+      <c r="M19" s="278"/>
     </row>
     <row r="20" spans="1:13" ht="52.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -8934,12 +8942,12 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="274" t="s">
+      <c r="A27" s="278" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="274"/>
-      <c r="C27" s="274"/>
-      <c r="D27" s="274"/>
+      <c r="B27" s="278"/>
+      <c r="C27" s="278"/>
+      <c r="D27" s="278"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
     </row>
@@ -8968,7 +8976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DBAA6-739A-4660-96E4-A6E1D48EB2A8}">
   <dimension ref="D2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -9040,7 +9048,7 @@
         <v>0.40721649484536082</v>
       </c>
       <c r="O4" s="227"/>
-      <c r="P4" s="277"/>
+      <c r="P4" s="254"/>
       <c r="Q4" s="243"/>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.25">
@@ -9070,7 +9078,7 @@
         <v>0.51546391752577314</v>
       </c>
       <c r="O5" s="35"/>
-      <c r="P5" s="278"/>
+      <c r="P5" s="255"/>
       <c r="Q5" s="243"/>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.25">
@@ -9100,7 +9108,7 @@
         <v>0.67010309278350511</v>
       </c>
       <c r="O6" s="35"/>
-      <c r="P6" s="278"/>
+      <c r="P6" s="255"/>
       <c r="Q6" s="243"/>
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.25">
@@ -9130,7 +9138,7 @@
         <v>0.82474226804123707</v>
       </c>
       <c r="O7" s="35"/>
-      <c r="P7" s="278"/>
+      <c r="P7" s="255"/>
       <c r="Q7" s="243"/>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.25">
@@ -9160,7 +9168,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="225"/>
-      <c r="P8" s="279"/>
+      <c r="P8" s="256"/>
     </row>
     <row r="9" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D9" s="224"/>

</xml_diff>

<commit_message>
Conclusion/Intro/Methodology left on writeup
</commit_message>
<xml_diff>
--- a/Assignments/Project4/Expectation Analysis.xlsx
+++ b/Assignments/Project4/Expectation Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE2A0D8-37C3-4174-A169-928BA097FD96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B79754-9048-4247-82EE-7601276204CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal" sheetId="12" r:id="rId1"/>
@@ -1658,7 +1658,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="282">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2384,6 +2384,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2705,8 +2706,8 @@
   </sheetPr>
   <dimension ref="A1:AM69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4826,7 +4827,7 @@
       <c r="AF32" s="119"/>
       <c r="AG32" s="119"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="140" t="s">
         <v>5</v>
       </c>
@@ -4854,7 +4855,7 @@
       </c>
       <c r="O33" s="119"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="141" t="s">
         <v>6</v>
       </c>
@@ -4882,7 +4883,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="142"/>
       <c r="B35" s="127"/>
       <c r="C35" s="127"/>
@@ -4892,7 +4893,7 @@
       <c r="K35" s="119"/>
       <c r="L35" s="69"/>
     </row>
-    <row r="36" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="143" t="s">
         <v>115</v>
       </c>
@@ -4940,7 +4941,7 @@
         <v>1900000</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="144" t="s">
         <v>2</v>
       </c>
@@ -4990,8 +4991,9 @@
         <f>O14*5000+Q14*5000</f>
         <v>45000</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T37" s="281"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="147" t="s">
         <v>3</v>
       </c>
@@ -5045,7 +5047,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="147" t="s">
         <v>4</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="147" t="s">
         <v>5</v>
       </c>
@@ -5133,7 +5135,7 @@
         <v>21600000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="149" t="s">
         <v>6</v>
       </c>
@@ -5178,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K42" s="119" t="s">
         <v>79</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>44800000</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="55"/>
       <c r="B43" s="55"/>
       <c r="C43" s="134"/>
@@ -5217,7 +5219,7 @@
         <v>18400000</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="127"/>
       <c r="B44" s="127"/>
       <c r="C44" s="134"/>
@@ -5238,7 +5240,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="127"/>
       <c r="B45" s="127"/>
       <c r="C45" s="134"/>
@@ -5259,7 +5261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="127"/>
       <c r="B46" s="127"/>
       <c r="C46" s="134"/>
@@ -5280,7 +5282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="127"/>
       <c r="B47" s="127"/>
       <c r="C47" s="134"/>
@@ -5293,7 +5295,7 @@
         <v>904720000</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="127"/>
       <c r="B48" s="127"/>
       <c r="C48" s="134"/>

</xml_diff>

<commit_message>
Tentatively done. Need to proofread and print
</commit_message>
<xml_diff>
--- a/Assignments/Project4/Expectation Analysis.xlsx
+++ b/Assignments/Project4/Expectation Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micah Hayden\Documents\AFIT\SP2019\CSCE 654 - Communications\Assignments\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B79754-9048-4247-82EE-7601276204CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03B92E4-A6DF-49D9-9F2C-FC7D1EE27891}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="700" xr2:uid="{DFA697D2-2C29-43C4-A322-5A73EA6783C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal" sheetId="12" r:id="rId1"/>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="131">
   <si>
     <t>Source</t>
   </si>
@@ -2315,6 +2315,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2384,7 +2385,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2707,7 +2707,7 @@
   <dimension ref="A1:AM69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,28 +2752,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="258" t="s">
+      <c r="J1" s="259" t="s">
         <v>124</v>
       </c>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
-      <c r="M1" s="258"/>
-      <c r="N1" s="258"/>
-      <c r="O1" s="258"/>
-      <c r="P1" s="258"/>
-      <c r="Q1" s="258"/>
-      <c r="R1" s="258"/>
-      <c r="S1" s="258"/>
-      <c r="T1" s="258"/>
-      <c r="U1" s="258"/>
-      <c r="V1" s="258"/>
-      <c r="W1" s="258"/>
-      <c r="X1" s="258"/>
-      <c r="Y1" s="258"/>
-      <c r="Z1" s="258"/>
-      <c r="AA1" s="258"/>
-      <c r="AB1" s="258"/>
-      <c r="AC1" s="258"/>
+      <c r="K1" s="259"/>
+      <c r="L1" s="259"/>
+      <c r="M1" s="259"/>
+      <c r="N1" s="259"/>
+      <c r="O1" s="259"/>
+      <c r="P1" s="259"/>
+      <c r="Q1" s="259"/>
+      <c r="R1" s="259"/>
+      <c r="S1" s="259"/>
+      <c r="T1" s="259"/>
+      <c r="U1" s="259"/>
+      <c r="V1" s="259"/>
+      <c r="W1" s="259"/>
+      <c r="X1" s="259"/>
+      <c r="Y1" s="259"/>
+      <c r="Z1" s="259"/>
+      <c r="AA1" s="259"/>
+      <c r="AB1" s="259"/>
+      <c r="AC1" s="259"/>
     </row>
     <row r="2" spans="1:38" s="116" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="95" t="s">
@@ -4035,16 +4035,16 @@
       <c r="AL18" s="119"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="260" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="262" t="s">
+      <c r="A19" s="261" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="263" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="263"/>
-      <c r="D19" s="263"/>
-      <c r="E19" s="263"/>
-      <c r="F19" s="264"/>
+      <c r="C19" s="264"/>
+      <c r="D19" s="264"/>
+      <c r="E19" s="264"/>
+      <c r="F19" s="265"/>
       <c r="G19" s="55"/>
       <c r="H19" s="55"/>
       <c r="I19" s="55"/>
@@ -4101,7 +4101,7 @@
       <c r="AL19" s="119"/>
     </row>
     <row r="20" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="261"/>
+      <c r="A20" s="262"/>
       <c r="B20" s="98" t="s">
         <v>2</v>
       </c>
@@ -4236,10 +4236,10 @@
         <v>2.0618556701030927E-2</v>
       </c>
       <c r="V21" s="119"/>
-      <c r="Z21" s="270" t="s">
+      <c r="Z21" s="271" t="s">
         <v>70</v>
       </c>
-      <c r="AA21" s="271"/>
+      <c r="AA21" s="272"/>
       <c r="AD21" s="119"/>
       <c r="AF21" s="119"/>
       <c r="AG21" s="119"/>
@@ -4682,16 +4682,16 @@
       <c r="AM27" s="119"/>
     </row>
     <row r="28" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="268" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="265" t="s">
+      <c r="A28" s="269" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="266" t="s">
         <v>123</v>
       </c>
-      <c r="C28" s="266"/>
-      <c r="D28" s="266"/>
-      <c r="E28" s="266"/>
-      <c r="F28" s="267"/>
+      <c r="C28" s="267"/>
+      <c r="D28" s="267"/>
+      <c r="E28" s="267"/>
+      <c r="F28" s="268"/>
       <c r="K28" s="143" t="s">
         <v>121</v>
       </c>
@@ -4717,7 +4717,7 @@
       <c r="AH28" s="119"/>
     </row>
     <row r="29" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="269"/>
+      <c r="A29" s="270"/>
       <c r="B29" s="139" t="s">
         <v>2</v>
       </c>
@@ -4777,13 +4777,13 @@
       <c r="F31" s="113">
         <v>50</v>
       </c>
-      <c r="K31" s="259" t="s">
+      <c r="K31" s="260" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="259"/>
-      <c r="M31" s="259"/>
-      <c r="N31" s="259"/>
-      <c r="O31" s="259"/>
+      <c r="L31" s="260"/>
+      <c r="M31" s="260"/>
+      <c r="N31" s="260"/>
+      <c r="O31" s="260"/>
       <c r="P31" s="119"/>
       <c r="Q31" s="119"/>
       <c r="AF31" s="119"/>
@@ -4991,7 +4991,7 @@
         <f>O14*5000+Q14*5000</f>
         <v>45000</v>
       </c>
-      <c r="T37" s="281"/>
+      <c r="T37" s="258"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="147" t="s">
@@ -6700,13 +6700,13 @@
       <c r="D15" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="259" t="s">
+      <c r="J15" s="260" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="259"/>
-      <c r="L15" s="259"/>
-      <c r="M15" s="259"/>
-      <c r="N15" s="259"/>
+      <c r="K15" s="260"/>
+      <c r="L15" s="260"/>
+      <c r="M15" s="260"/>
+      <c r="N15" s="260"/>
       <c r="O15" s="56"/>
       <c r="P15" s="56"/>
       <c r="Q15" s="56"/>
@@ -6812,16 +6812,16 @@
       <c r="AL17" s="56"/>
     </row>
     <row r="18" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="274" t="s">
+      <c r="A18" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="275"/>
-      <c r="D18" s="275"/>
-      <c r="E18" s="275"/>
-      <c r="F18" s="276"/>
+      <c r="C18" s="276"/>
+      <c r="D18" s="276"/>
+      <c r="E18" s="276"/>
+      <c r="F18" s="277"/>
       <c r="G18" s="55"/>
       <c r="H18" s="55"/>
       <c r="I18" s="55"/>
@@ -6844,7 +6844,7 @@
       <c r="AL18" s="56"/>
     </row>
     <row r="19" spans="1:39" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="273"/>
+      <c r="A19" s="274"/>
       <c r="B19" s="18" t="s">
         <v>2</v>
       </c>
@@ -8113,7 +8113,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G13"/>
+      <selection sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8127,34 +8127,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="274" t="s">
+      <c r="A1" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="275"/>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="276"/>
-      <c r="H1" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="274" t="s">
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="277"/>
+      <c r="H1" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="275"/>
-      <c r="K1" s="275"/>
-      <c r="L1" s="275"/>
-      <c r="M1" s="276"/>
-      <c r="O1" s="277" t="s">
+      <c r="J1" s="276"/>
+      <c r="K1" s="276"/>
+      <c r="L1" s="276"/>
+      <c r="M1" s="277"/>
+      <c r="O1" s="278" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="277"/>
-      <c r="Q1" s="277"/>
+      <c r="P1" s="278"/>
+      <c r="Q1" s="278"/>
     </row>
     <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="280"/>
+      <c r="A2" s="281"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="280"/>
+      <c r="H2" s="281"/>
       <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
@@ -8441,22 +8441,22 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="278" t="s">
+      <c r="A8" s="279" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="278"/>
-      <c r="C8" s="278"/>
-      <c r="D8" s="278"/>
-      <c r="E8" s="278"/>
-      <c r="F8" s="278"/>
-      <c r="H8" s="278" t="s">
+      <c r="B8" s="279"/>
+      <c r="C8" s="279"/>
+      <c r="D8" s="279"/>
+      <c r="E8" s="279"/>
+      <c r="F8" s="279"/>
+      <c r="H8" s="279" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="279"/>
-      <c r="J8" s="279"/>
-      <c r="K8" s="279"/>
-      <c r="L8" s="279"/>
-      <c r="M8" s="279"/>
+      <c r="I8" s="280"/>
+      <c r="J8" s="280"/>
+      <c r="K8" s="280"/>
+      <c r="L8" s="280"/>
+      <c r="M8" s="280"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="257"/>
@@ -8483,16 +8483,16 @@
       <c r="N9" s="223"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="274" t="s">
+      <c r="A10" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="275"/>
-      <c r="D10" s="275"/>
-      <c r="E10" s="275"/>
-      <c r="F10" s="276"/>
+      <c r="C10" s="276"/>
+      <c r="D10" s="276"/>
+      <c r="E10" s="276"/>
+      <c r="F10" s="277"/>
       <c r="G10" s="257"/>
       <c r="I10" s="223"/>
       <c r="J10" s="223"/>
@@ -8501,7 +8501,7 @@
       <c r="M10" s="223"/>
     </row>
     <row r="11" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="273"/>
+      <c r="A11" s="274"/>
       <c r="B11" s="18" t="s">
         <v>2</v>
       </c>
@@ -8544,16 +8544,16 @@
         <v>12000</v>
       </c>
       <c r="G12" s="257"/>
-      <c r="H12" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="274" t="s">
+      <c r="H12" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="275" t="s">
         <v>1</v>
       </c>
-      <c r="J12" s="275"/>
-      <c r="K12" s="275"/>
-      <c r="L12" s="275"/>
-      <c r="M12" s="276"/>
+      <c r="J12" s="276"/>
+      <c r="K12" s="276"/>
+      <c r="L12" s="276"/>
+      <c r="M12" s="277"/>
     </row>
     <row r="13" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -8575,7 +8575,7 @@
         <v>8200</v>
       </c>
       <c r="G13" s="257"/>
-      <c r="H13" s="280"/>
+      <c r="H13" s="281"/>
       <c r="I13" s="50" t="s">
         <v>2</v>
       </c>
@@ -8725,14 +8725,14 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="278" t="s">
+      <c r="A17" s="279" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="278"/>
-      <c r="C17" s="278"/>
-      <c r="D17" s="278"/>
-      <c r="E17" s="278"/>
-      <c r="F17" s="278"/>
+      <c r="B17" s="279"/>
+      <c r="C17" s="279"/>
+      <c r="D17" s="279"/>
+      <c r="E17" s="279"/>
+      <c r="F17" s="279"/>
       <c r="H17" s="10" t="s">
         <v>5</v>
       </c>
@@ -8796,14 +8796,14 @@
         <v>20</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="H19" s="278" t="s">
+      <c r="H19" s="279" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="278"/>
-      <c r="J19" s="278"/>
-      <c r="K19" s="278"/>
-      <c r="L19" s="278"/>
-      <c r="M19" s="278"/>
+      <c r="I19" s="279"/>
+      <c r="J19" s="279"/>
+      <c r="K19" s="279"/>
+      <c r="L19" s="279"/>
+      <c r="M19" s="279"/>
     </row>
     <row r="20" spans="1:13" ht="52.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
@@ -8944,12 +8944,12 @@
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="278" t="s">
+      <c r="A27" s="279" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="278"/>
-      <c r="C27" s="278"/>
-      <c r="D27" s="278"/>
+      <c r="B27" s="279"/>
+      <c r="C27" s="279"/>
+      <c r="D27" s="279"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
     </row>
@@ -8976,10 +8976,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DBAA6-739A-4660-96E4-A6E1D48EB2A8}">
-  <dimension ref="D2:Q36"/>
+  <dimension ref="D2:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="D4" sqref="D4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9593,7 +9593,7 @@
         <v>1.2886597938144331</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D33" s="189" t="s">
         <v>37</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>2.2353361945636623</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D34" s="174" t="s">
         <v>38</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>1.2886597938144331</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D35" s="189" t="s">
         <v>38</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>4.4706723891273246</v>
       </c>
     </row>
-    <row r="36" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D36" s="139" t="s">
         <v>40</v>
       </c>
@@ -9653,7 +9653,190 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="38" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="4:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="273" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="275" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="276"/>
+      <c r="G39" s="276"/>
+      <c r="H39" s="276"/>
+      <c r="I39" s="277"/>
+    </row>
+    <row r="40" spans="4:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="281"/>
+      <c r="E40" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="8">
+        <v>200</v>
+      </c>
+      <c r="G41" s="8">
+        <v>2500</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1000</v>
+      </c>
+      <c r="I41" s="9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="6">
+        <v>250</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>500</v>
+      </c>
+      <c r="H42" s="1">
+        <v>250</v>
+      </c>
+      <c r="I42" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>250</v>
+      </c>
+      <c r="F43" s="1">
+        <v>500</v>
+      </c>
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>500</v>
+      </c>
+      <c r="I43" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="1">
+        <v>250</v>
+      </c>
+      <c r="F44" s="1">
+        <v>500</v>
+      </c>
+      <c r="G44" s="1">
+        <v>500</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="11">
+        <v>250</v>
+      </c>
+      <c r="F45" s="1">
+        <v>200</v>
+      </c>
+      <c r="G45" s="1">
+        <v>250</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <f>SUM(E41:E45)</f>
+        <v>1000</v>
+      </c>
+      <c r="F46">
+        <f t="shared" ref="F46:I46" si="14">SUM(F41:F45)</f>
+        <v>1400</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="14"/>
+        <v>3750</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="14"/>
+        <v>2750</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="14"/>
+        <v>800</v>
+      </c>
+      <c r="J46">
+        <f>SUM(E46:I46)</f>
+        <v>9700</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="E47" s="243">
+        <f>E46/$J$46</f>
+        <v>0.10309278350515463</v>
+      </c>
+      <c r="F47" s="243">
+        <f t="shared" ref="F47:I47" si="15">F46/$J$46</f>
+        <v>0.14432989690721648</v>
+      </c>
+      <c r="G47" s="243">
+        <f t="shared" si="15"/>
+        <v>0.38659793814432991</v>
+      </c>
+      <c r="H47" s="243">
+        <f t="shared" si="15"/>
+        <v>0.28350515463917525</v>
+      </c>
+      <c r="I47" s="243">
+        <f t="shared" si="15"/>
+        <v>8.247422680412371E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:I39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>